<commit_message>
Reworking from Clusters to Bubbles
</commit_message>
<xml_diff>
--- a/tests/basicdiffusion/diffusion.xlsx
+++ b/tests/basicdiffusion/diffusion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="13640" yWindow="-17960" windowWidth="25040" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>x</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>temp</t>
   </si>
 </sst>
 </file>
@@ -100,8 +103,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -152,7 +157,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -175,6 +180,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -197,6 +203,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,7 +579,7 @@
   <dimension ref="C8:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:F19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -582,7 +589,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="1">
-        <v>30000000000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="9" spans="3:4">
@@ -595,90 +602,92 @@
     </row>
     <row r="10" spans="3:4">
       <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <f>D8*EXP(-D9/8.31446/1000)</f>
-        <v>8.5937016662607404E-9</v>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="3:4">
       <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <f>D8*EXP(-D9/8.31446/D10)</f>
+        <v>8.5937016662607413E-12</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4">
+      <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:4">
-      <c r="C13" t="s">
+    <row r="14" spans="3:4">
+      <c r="C14" t="s">
         <v>0</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="3:4">
-      <c r="C15" t="s">
+    <row r="16" spans="3:4">
+      <c r="C16" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6">
-      <c r="C17" t="s">
+      <c r="D16" s="1">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6">
-      <c r="C18" s="2">
-        <f>D15</f>
-        <v>100000</v>
-      </c>
-      <c r="D18" s="2">
-        <f>$D$11*(1-ERF(0,$D$13/SQRT(4*$D$10*C18)))</f>
-        <v>0.80939255148116862</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.80870310000000001</v>
-      </c>
-      <c r="F18" s="2">
-        <f>ABS(E18-D18)/D18*100</f>
-        <v>8.5181347407624786E-2</v>
       </c>
     </row>
     <row r="19" spans="3:6">
       <c r="C19" s="2">
-        <f>C18+$D$15</f>
-        <v>200000</v>
+        <f>D16</f>
+        <v>10000000</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" ref="D19:D22" si="0">$D$11*(1-ERF(0,$D$13/SQRT(4*$D$10*C19)))</f>
-        <v>0.86456892451322154</v>
+        <f>$D$12*(1-ERF(0,$D$14/SQRT(4*$D$11*C19)))</f>
+        <v>0.44559925342017581</v>
       </c>
       <c r="E19" s="2">
+        <v>0.80870310000000001</v>
+      </c>
+      <c r="F19" s="2">
+        <f>ABS(E19-D19)/D19*100</f>
+        <v>81.486637105614051</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="2">
+        <f>C19+$D$16</f>
+        <v>20000000</v>
+      </c>
+      <c r="D20" s="2">
+        <f>$D$12*(1-ERF(0,$D$14/SQRT(4*$D$11*C20)))</f>
+        <v>0.58963750525015812</v>
+      </c>
+      <c r="E20" s="2">
         <v>0.86431950000000002</v>
       </c>
-      <c r="F19" s="2">
-        <f t="shared" ref="F19:F22" si="1">ABS(E19-D19)/D19*100</f>
-        <v>2.8849581120666868E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6">
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2">
+        <f t="shared" ref="F20" si="0">ABS(E20-D20)/D20*100</f>
+        <v>46.584891955491535</v>
+      </c>
     </row>
     <row r="21" spans="3:6">
       <c r="C21" s="1"/>

</xml_diff>